<commit_message>
incorporating lab frags, starting comparative analyses across nurseries
</commit_message>
<xml_diff>
--- a/restoration_monitoring/data_raw/Nursery map.xlsx
+++ b/restoration_monitoring/data_raw/Nursery map.xlsx
@@ -77,14 +77,7 @@
 Print - tag needs to be printed</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A14">
-      <text>
-        <t xml:space="preserve">Do I need to put both tags even though there is only one fragment for this genotype at this location? @mwattswilson@gmail.com
-_Assigned to mwattswilson@gmail.com_
-	-Monique Bigler</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="A6">
+    <comment authorId="0" ref="A4">
       <text>
         <t xml:space="preserve">Current tag in nursery: Temp09
 	-Monique Bigler</t>
@@ -111,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="199">
   <si>
     <t>APRO04</t>
   </si>
@@ -509,6 +502,9 @@
     <t>n frags current</t>
   </si>
   <si>
+    <t>source</t>
+  </si>
+  <si>
     <t xml:space="preserve">Needs tag </t>
   </si>
   <si>
@@ -563,67 +559,64 @@
     <t>Action</t>
   </si>
   <si>
+    <t>Rope</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>A2/GB</t>
+  </si>
+  <si>
+    <t>Deep Nursery</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>Already there</t>
+  </si>
+  <si>
+    <t>Print</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
     <t>BS</t>
   </si>
   <si>
     <t>Glue</t>
   </si>
   <si>
-    <t>Rope</t>
-  </si>
-  <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>B9</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>B7</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>D7</t>
+    <t>Awaiting instruction</t>
   </si>
   <si>
     <t>OANN7</t>
-  </si>
-  <si>
-    <t>Deep Nursery</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <t>Print</t>
-  </si>
-  <si>
-    <t>Restock</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>A2/GB</t>
-  </si>
-  <si>
-    <t>ACER7</t>
   </si>
   <si>
     <t>Structure</t>
@@ -1096,11 +1089,11 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -3005,8 +2998,304 @@
         <v>194</v>
       </c>
     </row>
+    <row r="30">
+      <c r="B30" s="43"/>
+      <c r="C30" s="51" t="s">
+        <v>186</v>
+      </c>
+      <c r="K30" s="43"/>
+      <c r="L30" s="66" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" s="43"/>
+      <c r="C31" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="D31" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="F31" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="H31" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="K31" s="43"/>
+      <c r="M31" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="N31" s="68"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="65"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="53">
+        <v>1.0</v>
+      </c>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="F32" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="G32" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="H32" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="M32" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="N32" s="68"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="53">
+        <v>2.0</v>
+      </c>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="F33" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="G33" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="H33" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="K33" s="43"/>
+      <c r="L33" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="M33" s="52" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" s="53">
+        <v>3.0</v>
+      </c>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="F34" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="G34" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="H34" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="K34" s="53">
+        <v>1.0</v>
+      </c>
+      <c r="L34" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="M34" s="73" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" s="53">
+        <v>4.0</v>
+      </c>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="F35" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="G35" s="61"/>
+      <c r="H35" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="K35" s="53">
+        <v>2.0</v>
+      </c>
+      <c r="L35" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="M35" s="74"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="53">
+        <v>5.0</v>
+      </c>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="61"/>
+      <c r="H36" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="K36" s="53">
+        <v>3.0</v>
+      </c>
+      <c r="L36" s="74"/>
+      <c r="M36" s="73" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="53">
+        <v>6.0</v>
+      </c>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="F37" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="G37" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H37" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="K37" s="53">
+        <v>4.0</v>
+      </c>
+      <c r="L37" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="M37" s="74"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="53">
+        <v>7.0</v>
+      </c>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="F38" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="G38" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H38" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="K38" s="53">
+        <v>5.0</v>
+      </c>
+      <c r="L38" s="74"/>
+      <c r="M38" s="58" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" s="53">
+        <v>8.0</v>
+      </c>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="F39" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="G39" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H39" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="K39" s="53">
+        <v>6.0</v>
+      </c>
+      <c r="L39" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="M39" s="74"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="53">
+        <v>9.0</v>
+      </c>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="G40" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H40" s="60" t="s">
+        <v>195</v>
+      </c>
+      <c r="K40" s="53">
+        <v>7.0</v>
+      </c>
+      <c r="L40" s="75"/>
+      <c r="M40" s="58" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" s="43"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="65"/>
+      <c r="K41" s="53">
+        <v>8.0</v>
+      </c>
+      <c r="L41" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="M41" s="75"/>
+    </row>
+    <row r="42">
+      <c r="K42" s="53">
+        <v>9.0</v>
+      </c>
+      <c r="L42" s="75"/>
+      <c r="M42" s="58" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="24">
     <mergeCell ref="P14:U14"/>
     <mergeCell ref="W14:AB14"/>
     <mergeCell ref="Q15:S15"/>
@@ -3015,11 +3304,6 @@
     <mergeCell ref="Q16:S16"/>
     <mergeCell ref="X16:Z16"/>
     <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="J16:L16"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="P1:U1"/>
@@ -3027,6 +3311,15 @@
     <mergeCell ref="AD1:AI1"/>
     <mergeCell ref="I14:N14"/>
     <mergeCell ref="AD14:AI14"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="L30:Q30"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -5148,9 +5441,11 @@
         <v>131</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="42"/>
       <c r="F1" s="42"/>
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
@@ -5173,6 +5468,7 @@
       <c r="Y1" s="42"/>
       <c r="Z1" s="42"/>
       <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
     </row>
     <row r="2">
       <c r="A2" s="41" t="s">
@@ -5181,6 +5477,9 @@
       <c r="B2" s="41">
         <v>4.0</v>
       </c>
+      <c r="D2" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="41" t="s">
@@ -5189,6 +5488,9 @@
       <c r="B3" s="41">
         <v>4.0</v>
       </c>
+      <c r="D3" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="41" t="s">
@@ -5197,6 +5499,9 @@
       <c r="B4" s="41">
         <v>4.0</v>
       </c>
+      <c r="D4" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="41" t="s">
@@ -5205,6 +5510,9 @@
       <c r="B5" s="41">
         <v>4.0</v>
       </c>
+      <c r="D5" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="41" t="s">
@@ -5213,6 +5521,9 @@
       <c r="B6" s="41">
         <v>4.0</v>
       </c>
+      <c r="D6" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="41" t="s">
@@ -5221,6 +5532,9 @@
       <c r="B7" s="41">
         <v>4.0</v>
       </c>
+      <c r="D7" s="41" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="41" t="s">
@@ -5229,6 +5543,9 @@
       <c r="B8" s="41">
         <v>4.0</v>
       </c>
+      <c r="D8" s="41" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="41" t="s">
@@ -5237,6 +5554,9 @@
       <c r="B9" s="41">
         <v>4.0</v>
       </c>
+      <c r="D9" s="41" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="41" t="s">
@@ -5245,6 +5565,9 @@
       <c r="B10" s="41">
         <v>3.0</v>
       </c>
+      <c r="D10" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="41" t="s">
@@ -5253,6 +5576,9 @@
       <c r="B11" s="41">
         <v>4.0</v>
       </c>
+      <c r="D11" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="41" t="s">
@@ -5261,6 +5587,9 @@
       <c r="B12" s="41">
         <v>4.0</v>
       </c>
+      <c r="D12" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="41" t="s">
@@ -5269,6 +5598,9 @@
       <c r="B13" s="41">
         <v>4.0</v>
       </c>
+      <c r="D13" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="41" t="s">
@@ -5277,6 +5609,9 @@
       <c r="B14" s="41">
         <v>4.0</v>
       </c>
+      <c r="D14" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="41" t="s">
@@ -5285,6 +5620,9 @@
       <c r="B15" s="41">
         <v>4.0</v>
       </c>
+      <c r="D15" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="41" t="s">
@@ -5295,7 +5633,10 @@
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="41" t="s">
-        <v>132</v>
+        <v>49</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="17">
@@ -5305,6 +5646,9 @@
       <c r="B17" s="41">
         <v>4.0</v>
       </c>
+      <c r="D17" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="41" t="s">
@@ -5313,6 +5657,9 @@
       <c r="B18" s="41">
         <v>4.0</v>
       </c>
+      <c r="D18" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="41" t="s">
@@ -5321,6 +5668,9 @@
       <c r="B19" s="41">
         <v>4.0</v>
       </c>
+      <c r="D19" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="41" t="s">
@@ -5329,6 +5679,9 @@
       <c r="B20" s="41">
         <v>4.0</v>
       </c>
+      <c r="D20" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="41" t="s">
@@ -5337,6 +5690,9 @@
       <c r="B21" s="41">
         <v>4.0</v>
       </c>
+      <c r="D21" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="41" t="s">
@@ -5345,13 +5701,19 @@
       <c r="B22" s="41">
         <v>4.0</v>
       </c>
+      <c r="D22" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B23" s="41">
         <v>4.0</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24">
@@ -5361,6 +5723,9 @@
       <c r="B24" s="41">
         <v>4.0</v>
       </c>
+      <c r="D24" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="41" t="s">
@@ -5369,6 +5734,9 @@
       <c r="B25" s="41">
         <v>4.0</v>
       </c>
+      <c r="D25" s="41" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="41" t="s">
@@ -5377,6 +5745,9 @@
       <c r="B26" s="41">
         <v>4.0</v>
       </c>
+      <c r="D26" s="41" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="41" t="s">
@@ -5384,6 +5755,9 @@
       </c>
       <c r="B27" s="41">
         <v>4.0</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -5403,13 +5777,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
@@ -5438,12 +5812,12 @@
     </row>
     <row r="2">
       <c r="A2" s="41" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="41" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B3" s="41"/>
       <c r="C3" s="41" t="s">
@@ -5452,37 +5826,37 @@
     </row>
     <row r="4">
       <c r="A4" s="41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="41" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="41" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="41" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="41" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="41" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="41" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B10" s="41"/>
       <c r="C10" s="41" t="s">
@@ -5508,28 +5882,32 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="15.75"/>
+    <col customWidth="1" min="1" max="1" width="8.63"/>
+    <col customWidth="1" min="2" max="2" width="15.75"/>
+    <col customWidth="1" min="3" max="3" width="8.25"/>
+    <col customWidth="1" min="4" max="4" width="15.88"/>
+    <col customWidth="1" min="5" max="5" width="15.75"/>
     <col customWidth="1" min="6" max="6" width="16.13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>135</v>
-      </c>
       <c r="F1" s="47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
@@ -5602,248 +5980,168 @@
     </row>
     <row r="2">
       <c r="A2" s="41" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="48">
+        <v>151</v>
+      </c>
+      <c r="C2" s="41">
         <v>1.0</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="F2" s="41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="42"/>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
-      <c r="AG2" s="42"/>
-      <c r="AH2" s="42"/>
-      <c r="AI2" s="42"/>
-      <c r="AJ2" s="42"/>
-      <c r="AK2" s="42"/>
-      <c r="AL2" s="42"/>
-      <c r="AM2" s="42"/>
-      <c r="AN2" s="42"/>
-      <c r="AO2" s="42"/>
-      <c r="AP2" s="42"/>
-      <c r="AQ2" s="42"/>
-      <c r="AR2" s="42"/>
-      <c r="AS2" s="42"/>
-      <c r="AT2" s="42"/>
-      <c r="AU2" s="42"/>
-      <c r="AV2" s="42"/>
-      <c r="AW2" s="42"/>
-      <c r="AX2" s="42"/>
-      <c r="AY2" s="42"/>
-      <c r="AZ2" s="42"/>
-      <c r="BA2" s="42"/>
-      <c r="BB2" s="42"/>
-      <c r="BC2" s="42"/>
-      <c r="BD2" s="42"/>
-      <c r="BE2" s="42"/>
-      <c r="BF2" s="42"/>
-      <c r="BG2" s="42"/>
-      <c r="BH2" s="42"/>
-      <c r="BI2" s="42"/>
-      <c r="BJ2" s="42"/>
-      <c r="BK2" s="42"/>
-      <c r="BL2" s="42"/>
-      <c r="BM2" s="42"/>
-      <c r="BN2" s="42"/>
-      <c r="BO2" s="42"/>
-      <c r="BP2" s="42"/>
-      <c r="BQ2" s="42"/>
-      <c r="BR2" s="42"/>
-      <c r="BS2" s="42"/>
-      <c r="BT2" s="42"/>
-      <c r="BU2" s="42"/>
-      <c r="BV2" s="42"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="48">
+      <c r="C3" s="41">
         <v>1.0</v>
       </c>
-      <c r="D3" s="43" t="s">
-        <v>72</v>
+      <c r="D3" s="41" t="s">
+        <v>89</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="F3" s="41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="K3" s="48"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="48">
+      <c r="C4" s="41">
         <v>1.0</v>
       </c>
-      <c r="D4" s="43" t="s">
-        <v>72</v>
+      <c r="D4" s="41" t="s">
+        <v>89</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="I4" s="43"/>
-      <c r="K4" s="48"/>
+        <v>152</v>
+      </c>
+      <c r="J4" s="48"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="43"/>
     </row>
     <row r="5">
       <c r="A5" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="41">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="48">
-        <v>1.0</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5" s="43"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="43"/>
     </row>
     <row r="6">
       <c r="A6" s="41" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="41">
         <v>1.0</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="J6" s="49"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="43"/>
+        <v>152</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="41" t="s">
-        <v>154</v>
+        <v>70</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C7" s="41">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="41" t="s">
-        <v>154</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="E7" s="41"/>
       <c r="F7" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="41" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C8" s="41">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>72</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="41" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C9" s="41">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D9" s="41" t="s">
         <v>72</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="41" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="C10" s="41">
         <v>1.0</v>
@@ -5852,38 +6150,38 @@
         <v>72</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="41" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C11" s="41">
         <v>1.0</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="41" t="s">
-        <v>160</v>
+        <v>12</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C12" s="41">
         <v>1.0</v>
@@ -5892,78 +6190,87 @@
         <v>72</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="41" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="41">
         <v>1.0</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="F14" s="41" t="s">
-        <v>153</v>
-      </c>
+      <c r="I14" s="43"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="43"/>
     </row>
     <row r="15">
       <c r="A15" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C15" s="41">
+        <v>81</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="49">
         <v>1.0</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="49" t="s">
         <v>72</v>
       </c>
       <c r="E15" s="41" t="s">
         <v>107</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>153</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="I15" s="43"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="43"/>
     </row>
     <row r="16">
       <c r="A16" s="41" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C16" s="41">
         <v>1.0</v>
@@ -5972,89 +6279,113 @@
         <v>72</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="41" t="s">
-        <v>38</v>
+        <v>166</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C17" s="41">
         <v>1.0</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>163</v>
+        <v>72</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>166</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>164</v>
+        <v>152</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="41" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C18" s="41">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="E18" s="41"/>
+        <v>72</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="F18" s="41" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="41" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C19" s="41">
         <v>2.0</v>
       </c>
       <c r="D19" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="E19" s="41"/>
+        <v>72</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="F19" s="41" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="41" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C20" s="41">
         <v>2.0</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="E20" s="41"/>
+        <v>72</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>73</v>
+      </c>
       <c r="F20" s="41" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="41" t="s">
-        <v>37</v>
+        <v>170</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C21" s="41">
         <v>1.0</v>
@@ -6066,35 +6397,41 @@
         <v>107</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>153</v>
+        <v>168</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="41" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C22" s="41">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D22" s="41" t="s">
         <v>72</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>153</v>
+        <v>168</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="41" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="C23" s="41">
         <v>1.0</v>
@@ -6103,18 +6440,21 @@
         <v>72</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>153</v>
+        <v>168</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="41" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="C24" s="41">
         <v>1.0</v>
@@ -6126,15 +6466,18 @@
         <v>73</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>153</v>
+        <v>168</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="41" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C25" s="41">
         <v>1.0</v>
@@ -6143,18 +6486,18 @@
         <v>72</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="41" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C26" s="41">
         <v>1.0</v>
@@ -6163,61 +6506,65 @@
         <v>72</v>
       </c>
       <c r="E26" s="41" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="41" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C27" s="41">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D27" s="41" t="s">
         <v>72</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="41" t="s">
-        <v>81</v>
+      <c r="A28" s="43" t="s">
+        <v>85</v>
       </c>
       <c r="B28" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D28" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="49">
+        <v>1.0</v>
+      </c>
+      <c r="D28" s="43" t="s">
         <v>72</v>
       </c>
       <c r="E28" s="41" t="s">
         <v>73</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>153</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="K28" s="49"/>
     </row>
     <row r="29">
       <c r="A29" s="41" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="C29" s="41">
-        <v>2.0</v>
+        <v>167</v>
+      </c>
+      <c r="C29" s="49">
+        <v>1.0</v>
       </c>
       <c r="D29" s="41" t="s">
         <v>72</v>
@@ -6226,716 +6573,114 @@
         <v>73</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>153</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="H29" s="42"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="42"/>
+      <c r="U29" s="42"/>
+      <c r="V29" s="42"/>
+      <c r="W29" s="42"/>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="42"/>
+      <c r="Z29" s="42"/>
+      <c r="AA29" s="42"/>
+      <c r="AB29" s="42"/>
+      <c r="AC29" s="42"/>
+      <c r="AD29" s="42"/>
+      <c r="AE29" s="42"/>
+      <c r="AF29" s="42"/>
+      <c r="AG29" s="42"/>
+      <c r="AH29" s="42"/>
+      <c r="AI29" s="42"/>
+      <c r="AJ29" s="42"/>
+      <c r="AK29" s="42"/>
+      <c r="AL29" s="42"/>
+      <c r="AM29" s="42"/>
+      <c r="AN29" s="42"/>
+      <c r="AO29" s="42"/>
+      <c r="AP29" s="42"/>
+      <c r="AQ29" s="42"/>
+      <c r="AR29" s="42"/>
+      <c r="AS29" s="42"/>
+      <c r="AT29" s="42"/>
+      <c r="AU29" s="42"/>
+      <c r="AV29" s="42"/>
+      <c r="AW29" s="42"/>
+      <c r="AX29" s="42"/>
+      <c r="AY29" s="42"/>
+      <c r="AZ29" s="42"/>
+      <c r="BA29" s="42"/>
+      <c r="BB29" s="42"/>
+      <c r="BC29" s="42"/>
+      <c r="BD29" s="42"/>
+      <c r="BE29" s="42"/>
+      <c r="BF29" s="42"/>
+      <c r="BG29" s="42"/>
+      <c r="BH29" s="42"/>
+      <c r="BI29" s="42"/>
+      <c r="BJ29" s="42"/>
+      <c r="BK29" s="42"/>
+      <c r="BL29" s="42"/>
+      <c r="BM29" s="42"/>
+      <c r="BN29" s="42"/>
+      <c r="BO29" s="42"/>
+      <c r="BP29" s="42"/>
+      <c r="BQ29" s="42"/>
+      <c r="BR29" s="42"/>
+      <c r="BS29" s="42"/>
+      <c r="BT29" s="42"/>
+      <c r="BU29" s="42"/>
+      <c r="BV29" s="42"/>
     </row>
     <row r="30">
-      <c r="A30" s="41" t="s">
-        <v>12</v>
+      <c r="A30" s="43" t="s">
+        <v>78</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="41">
+        <v>167</v>
+      </c>
+      <c r="C30" s="49">
         <v>1.0</v>
       </c>
-      <c r="D30" s="41" t="s">
+      <c r="D30" s="43" t="s">
         <v>72</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>166</v>
+        <v>73</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C31" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D31" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D32" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="F32" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C33" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D33" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="F33" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C34" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D34" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" s="41" t="s">
+      <c r="G30" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="F34" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D35" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="F35" s="41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="B36" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C36" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C37" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D37" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F37" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F38" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F39" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F40" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="41" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D41" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F41" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="B42" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C42" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D42" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F42" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C43" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D43" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F43" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C44" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D44" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F44" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C45" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D45" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F45" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C46" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D46" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F46" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C47" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D47" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F47" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B48" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D48" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F48" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D49" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F49" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C50" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D50" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F50" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D51" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F51" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B52" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C52" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D52" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F52" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C53" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D53" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F53" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D54" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F54" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C55" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D55" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F55" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C56" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D56" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F56" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C57" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D57" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F57" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C58" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D58" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F58" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="B59" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D59" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F59" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C60" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D60" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F60" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C61" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D61" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F61" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B62" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C62" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D62" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F62" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C63" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D63" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F63" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C64" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D64" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F64" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="B65" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C65" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D65" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F65" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C66" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D66" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F66" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C67" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D67" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F67" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B68" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C68" s="41">
-        <v>1.0</v>
-      </c>
-      <c r="D68" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F68" s="41" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C69" s="41">
-        <v>2.0</v>
-      </c>
-      <c r="D69" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="F69" s="41" t="s">
-        <v>164</v>
-      </c>
+      <c r="I30" s="43"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="43"/>
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F69">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F30">
       <formula1>"Glue,Add,Print"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D69">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D30">
       <formula1>"Cades,Deep Nursery,TPB,York,Lab,Restock"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B69">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B30">
       <formula1>"BS,DB,Rope,Tree"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>